<commit_message>
revert and update Capberechnung
</commit_message>
<xml_diff>
--- a/libraries/Adafruit_MPR121-master/Cap.xlsx
+++ b/libraries/Adafruit_MPR121-master/Cap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>C</t>
   </si>
@@ -49,6 +49,39 @@
   </si>
   <si>
     <t>Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstand </t>
+  </si>
+  <si>
+    <t>Platte X</t>
+  </si>
+  <si>
+    <t>Platte Y</t>
+  </si>
+  <si>
+    <t>epsilon</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
+  <si>
+    <t>trocken</t>
+  </si>
+  <si>
+    <t>feucht</t>
+  </si>
+  <si>
+    <t>Wasser</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -104,6 +137,165 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$O$53:$O$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$P$53:$P$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="126532608"/>
+        <c:axId val="126530688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="126532608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="126530688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="126530688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="126532608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,13 +585,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:S57"/>
+  <dimension ref="C3:S72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -2507,8 +2702,14 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>20</v>
+      </c>
+      <c r="Q48">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D49">
         <v>3</v>
       </c>
@@ -2532,8 +2733,14 @@
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>80</v>
+      </c>
+      <c r="Q49">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D50">
         <v>4</v>
       </c>
@@ -2558,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D51">
         <v>5</v>
       </c>
@@ -2583,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D52">
         <v>6</v>
       </c>
@@ -2608,7 +2815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D53">
         <v>7</v>
       </c>
@@ -2632,8 +2839,14 @@
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>20</v>
+      </c>
+      <c r="P53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D54">
         <v>8</v>
       </c>
@@ -2657,8 +2870,14 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>95</v>
+      </c>
+      <c r="P54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>9</v>
       </c>
@@ -2683,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D56">
         <v>10</v>
       </c>
@@ -2708,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>11</v>
       </c>
@@ -2730,6 +2949,148 @@
       </c>
       <c r="I57">
         <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P60">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P61">
+        <f>-0.3733 *P60 +87.467</f>
+        <v>78.134500000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64">
+        <v>70</v>
+      </c>
+      <c r="F64" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64">
+        <f>E64/1000</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64">
+        <f>G65*G66</f>
+        <v>2.5000000000000005E-3</v>
+      </c>
+      <c r="J64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65">
+        <v>50</v>
+      </c>
+      <c r="F65" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65">
+        <f t="shared" ref="G65:G66" si="17">E65/1000</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66">
+        <v>50</v>
+      </c>
+      <c r="F66" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="17"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67">
+        <f>8.85*10^-12</f>
+        <v>8.8499999999999988E-12</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>19</v>
+      </c>
+      <c r="H69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>3.9</v>
+      </c>
+      <c r="G70">
+        <v>29</v>
+      </c>
+      <c r="H70">
+        <v>80</v>
+      </c>
+      <c r="K70">
+        <f>G70-0.3733*5</f>
+        <v>27.133500000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <f>F70*$E$67*$I$64/$G$64</f>
+        <v>1.2326785714285715E-12</v>
+      </c>
+      <c r="G71">
+        <f>G70*$E$67*$I$64/$G$64</f>
+        <v>9.1660714285714286E-12</v>
+      </c>
+      <c r="H71">
+        <f>H70*$E$67*$I$64/$G$64</f>
+        <v>2.5285714285714286E-11</v>
+      </c>
+      <c r="I71" t="s">
+        <v>21</v>
+      </c>
+      <c r="K71">
+        <f>K70*$E$67*$I$64/$G$64</f>
+        <v>8.5761241071428576E-12</v>
+      </c>
+    </row>
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f>F71*10^12</f>
+        <v>1.2326785714285715</v>
+      </c>
+      <c r="G72">
+        <f t="shared" ref="G72:H72" si="18">G71*10^12</f>
+        <v>9.1660714285714278</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="18"/>
+        <v>25.285714285714285</v>
+      </c>
+      <c r="I72" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2740,6 +3101,7 @@
     <mergeCell ref="G44:H44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>